<commit_message>
Account for custom cell format
</commit_message>
<xml_diff>
--- a/inst/extdata/ex.data.xlsx
+++ b/inst/extdata/ex.data.xlsx
@@ -78,7 +78,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="170" formatCode="m/d/yy\ h:mm"/>
+    <numFmt numFmtId="171" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -161,7 +161,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>

<commit_message>
Fix NA with blank enteries
</commit_message>
<xml_diff>
--- a/inst/extdata/ex.data.xlsx
+++ b/inst/extdata/ex.data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WORK\JFisher\Software\RSurvey\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software\RSurvey\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
   <si>
     <t>A1</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     NA</t>
   </si>
   <si>
     <t>A4</t>
@@ -476,7 +473,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -497,42 +496,42 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -904,7 +903,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H12" s="7">
         <v>2.8999999999999998E-3</v>
@@ -944,7 +943,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H13" s="7">
         <v>2.9000000000000001E-2</v>
@@ -1160,7 +1159,7 @@
         <v>0.49965277777777778</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
@@ -2366,7 +2365,7 @@
         <v>0.50274305555555554</v>
       </c>
       <c r="O50" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More defaults for date-time cell formats
</commit_message>
<xml_diff>
--- a/inst/extdata/ex.data.xlsx
+++ b/inst/extdata/ex.data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software\RSurvey\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WORK\JFisher\Software\RSurvey\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>A1</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Logical</t>
-  </si>
-  <si>
-    <t>T POSIXct</t>
   </si>
   <si>
     <t>Character</t>
@@ -60,10 +57,16 @@
     <t>Z numeric, m</t>
   </si>
   <si>
-    <t>Date character</t>
+    <t>T date-time</t>
   </si>
   <si>
-    <t>Time character</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     NA</t>
   </si>
 </sst>
 </file>
@@ -473,9 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -496,29 +497,29 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
@@ -531,7 +532,7 @@
         <v>14</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -903,7 +904,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H12" s="7">
         <v>2.8999999999999998E-3</v>
@@ -943,7 +944,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H13" s="7">
         <v>2.9000000000000001E-2</v>

</xml_diff>